<commit_message>
add location to input_data.xlsx
</commit_message>
<xml_diff>
--- a/input_data.xlsx
+++ b/input_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jake/code/syseng-takehome/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A915AFE3-1D11-F44C-A0C3-4A4E9B747144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2405327-1BA6-0C43-9BD9-5AFF44E75D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9280" yWindow="2820" windowWidth="28040" windowHeight="17440" xr2:uid="{68A77180-E0E1-654D-BDA6-A8B9E21F164D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="67">
   <si>
     <t>Company Name</t>
   </si>
@@ -227,6 +227,15 @@
   </si>
   <si>
     <t>125OO</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>TN</t>
   </si>
 </sst>
 </file>
@@ -593,893 +602,1046 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279D27DB-756C-7D40-8D92-8B9A399B46BC}">
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.5" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" customWidth="1"/>
+    <col min="1" max="2" width="41.5" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>44656</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>44902</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>15000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>44656</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>44902</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>12000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>44656</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>44902</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>10000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>44718</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>44902</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>12000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>44718</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>44902</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>12000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>44718</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>44902</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>15000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>44748</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>44902</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>16500</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>44508</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>44873</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>12000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>44508</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>44873</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>12000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>44508</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>44873</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>12000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>44508</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <v>44873</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>12000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>44508</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <v>44873</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>12000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>44541</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E14" s="2">
         <v>44873</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>16000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
       <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>44566</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15" s="2">
         <v>44873</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>16000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>44566</v>
       </c>
-      <c r="D16" s="2">
+      <c r="E16" s="2">
         <v>44873</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>16500</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>44566</v>
       </c>
-      <c r="D17" s="2">
+      <c r="E17" s="2">
         <v>44873</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>14000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>44566</v>
       </c>
-      <c r="D18" s="2">
+      <c r="E18" s="2">
         <v>44873</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>18000</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
       <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="2">
+      <c r="E19" s="2">
         <v>44835</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>14000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
       <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="2">
+      <c r="E20" s="2">
         <v>44835</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>14000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
       <c r="B21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="2">
+      <c r="E21" s="2">
         <v>44835</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>14000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="2">
+      <c r="E22" s="2">
         <v>44835</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>15000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>8</v>
       </c>
       <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="2">
+      <c r="D23" s="2">
         <v>44440</v>
       </c>
-      <c r="D23" s="2">
+      <c r="E23" s="2">
         <v>44805</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>8000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>8</v>
       </c>
       <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="2">
+      <c r="D24" s="2">
         <v>44440</v>
       </c>
-      <c r="D24" s="2">
+      <c r="E24" s="2">
         <v>44805</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>23000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>8</v>
       </c>
       <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="2">
+      <c r="D25" s="2">
         <v>44440</v>
       </c>
-      <c r="D25" s="2">
+      <c r="E25" s="2">
         <v>44805</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>12000</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>8</v>
       </c>
       <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="2">
+      <c r="D26" s="2">
         <v>44440</v>
       </c>
-      <c r="D26" s="2">
+      <c r="E26" s="2">
         <v>44805</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>24000</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>8</v>
       </c>
       <c r="B27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="2">
+      <c r="D27" s="2">
         <v>44470</v>
       </c>
-      <c r="D27" s="2">
+      <c r="E27" s="2">
         <v>44805</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>12000</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>8</v>
       </c>
       <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="1">
+      <c r="D28" s="1">
         <v>44501</v>
       </c>
-      <c r="D28" s="2">
+      <c r="E28" s="2">
         <v>44805</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>15000</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
       <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="1">
+      <c r="D29" s="1">
         <v>44531</v>
       </c>
-      <c r="D29" s="2">
+      <c r="E29" s="2">
         <v>44805</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>15000</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>9</v>
       </c>
       <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="1">
+      <c r="D30" s="1">
         <v>44562</v>
       </c>
-      <c r="D30" s="2">
+      <c r="E30" s="2">
         <v>44896</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>10000</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>9</v>
       </c>
       <c r="B31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="1">
+      <c r="D31" s="1">
         <v>44562</v>
       </c>
-      <c r="D31" s="2">
+      <c r="E31" s="2">
         <v>44896</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>11000</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>9</v>
       </c>
       <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="1">
+      <c r="D32" s="1">
         <v>44593</v>
       </c>
-      <c r="D32" s="2">
+      <c r="E32" s="2">
         <v>44896</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>9000</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>9</v>
       </c>
       <c r="B33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="1">
+      <c r="D33" s="1">
         <v>44593</v>
       </c>
-      <c r="D33" s="2">
+      <c r="E33" s="2">
         <v>44896</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>12000</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>9</v>
       </c>
       <c r="B34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="1">
+      <c r="D34" s="1">
         <v>44593</v>
       </c>
-      <c r="D34" s="2">
+      <c r="E34" s="2">
         <v>44896</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>11000</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>9</v>
       </c>
       <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="1">
+      <c r="D35" s="1">
         <v>44593</v>
       </c>
-      <c r="D35" s="2">
+      <c r="E35" s="2">
         <v>44896</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>10000</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>9</v>
       </c>
       <c r="B36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="1">
+      <c r="D36" s="1">
         <v>44621</v>
       </c>
-      <c r="D36" s="2">
+      <c r="E36" s="2">
         <v>44896</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>9000</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>9</v>
       </c>
       <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="1">
+      <c r="D37" s="1">
         <v>44621</v>
       </c>
-      <c r="D37" s="2">
+      <c r="E37" s="2">
         <v>44896</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>11500</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>9</v>
       </c>
       <c r="B38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="1">
+      <c r="D38" s="1">
         <v>44656</v>
       </c>
-      <c r="D38" s="2">
+      <c r="E38" s="2">
         <v>44896</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>10500</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>9</v>
       </c>
       <c r="B39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" t="s">
         <v>47</v>
       </c>
-      <c r="C39" s="1">
+      <c r="D39" s="1">
         <v>44656</v>
       </c>
-      <c r="D39" s="2">
+      <c r="E39" s="2">
         <v>44896</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>12500</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>60</v>
       </c>
       <c r="B40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="2">
+      <c r="D40" s="2">
         <v>44378</v>
       </c>
-      <c r="D40" s="2">
+      <c r="E40" s="2">
         <v>44743</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>10000</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>60</v>
       </c>
       <c r="B41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="2">
+      <c r="D41" s="2">
         <v>44378</v>
       </c>
-      <c r="D41" s="2">
+      <c r="E41" s="2">
         <v>44743</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>10000</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>60</v>
       </c>
       <c r="B42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" t="s">
         <v>50</v>
       </c>
-      <c r="C42" s="2">
+      <c r="D42" s="2">
         <v>44378</v>
       </c>
-      <c r="D42" s="2">
+      <c r="E42" s="2">
         <v>44743</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>10000</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>60</v>
       </c>
       <c r="B43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" t="s">
         <v>51</v>
       </c>
-      <c r="C43" s="2">
+      <c r="D43" s="2">
         <v>44378</v>
       </c>
-      <c r="D43" s="2">
+      <c r="E43" s="2">
         <v>44743</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>10000</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>60</v>
       </c>
       <c r="B44" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="2">
+      <c r="D44" s="2">
         <v>44378</v>
       </c>
-      <c r="D44" s="2">
+      <c r="E44" s="2">
         <v>44743</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>10000</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>60</v>
       </c>
       <c r="B45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="2">
+      <c r="D45" s="2">
         <v>44378</v>
       </c>
-      <c r="D45" s="2">
+      <c r="E45" s="2">
         <v>44743</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>10000</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>60</v>
       </c>
       <c r="B46" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="2">
+      <c r="D46" s="2">
         <v>44378</v>
       </c>
-      <c r="D46" s="2">
+      <c r="E46" s="2">
         <v>44743</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>10000</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>60</v>
       </c>
       <c r="B47" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" t="s">
         <v>55</v>
       </c>
-      <c r="C47" s="2">
+      <c r="D47" s="2">
         <v>44378</v>
       </c>
-      <c r="D47" s="2">
+      <c r="E47" s="2">
         <v>44743</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>10000</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>60</v>
       </c>
       <c r="B48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="2">
+      <c r="D48" s="2">
         <v>44378</v>
       </c>
-      <c r="D48" s="2">
+      <c r="E48" s="2">
         <v>44743</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>10000</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>60</v>
       </c>
       <c r="B49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" t="s">
         <v>57</v>
       </c>
-      <c r="C49" s="2">
+      <c r="D49" s="2">
         <v>44561</v>
       </c>
-      <c r="D49" s="2">
+      <c r="E49" s="2">
         <v>44743</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>10000</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>61</v>
       </c>
       <c r="B50" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" t="s">
         <v>58</v>
       </c>
-      <c r="C50" s="1">
+      <c r="D50" s="1">
         <v>44440</v>
       </c>
-      <c r="D50" s="1">
+      <c r="E50" s="1">
         <v>44805</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="F50" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>61</v>
       </c>
       <c r="B51" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" t="s">
         <v>59</v>
       </c>
-      <c r="C51" s="1">
+      <c r="D51" s="1">
         <v>44440</v>
       </c>
-      <c r="D51" s="1">
+      <c r="E51" s="1">
         <v>44805</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="F51" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E52" s="4"/>
-    </row>
-    <row r="1048576" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D1048576" s="2"/>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F52" s="4"/>
+    </row>
+    <row r="1048576" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E1048576" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>